<commit_message>
feat: update rank xlsx
增加被对应段位击败减分字段
</commit_message>
<xml_diff>
--- a/battleworld/Excel/Rank_段位表.xlsx
+++ b/battleworld/Excel/Rank_段位表.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MetaWorldSaved\Saved\MetaWorld\Project\Edit\Dragonverse\battleworld\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\battleworld\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A006E9-7B19-46CF-BF97-790942760DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DB8A58-FA66-4F02-A8FE-338AA8CF4894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>int</t>
   </si>
@@ -79,10 +79,6 @@
   </si>
   <si>
     <t>所需积分</t>
-  </si>
-  <si>
-    <t>（被）击败不同段位（丢）得分
-练气|筑基|金丹|元婴|化神|炼虚|合体</t>
   </si>
   <si>
     <t>段位奖励商店ID
@@ -147,6 +143,36 @@
   </si>
   <si>
     <t>4|6|9|10|12|15|18</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>击败不同段位得分
+练气|筑基|金丹|元婴|化神|炼虚|合体</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>被不同段位击败丢分
+练气|筑基|金丹|元婴|化神|炼虚|合体</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>rankIntegralReduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0|0|0|0|0|0|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>25|23|15|12|10|8|5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>20|18|10|9|6|4|2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>23|20|12|10|9|6|4</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -536,20 +562,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="5" max="6" width="31.140625" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,19 +592,22 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -595,19 +624,22 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -621,202 +653,226 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C4" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5">
+      <c r="F5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5">
         <v>296288</v>
       </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
       <c r="I5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="1">
+        <v>200</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1">
-        <v>500</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6">
+      <c r="F6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6">
         <v>296289</v>
       </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
       <c r="I6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1">
+        <v>500</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="7">
         <v>4001</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>296292</v>
       </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
       <c r="I7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D8" s="1">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="8">
+        <v>35</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="8">
         <v>4002</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>296285</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>1</v>
       </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D9" s="1">
         <v>2000</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="9">
+        <v>32</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="9">
         <v>4003</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>296281</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>2</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="8"/>
-      <c r="H10" s="2"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="8"/>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="1"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E15" s="2"/>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G19" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H19" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>